<commit_message>
Cập nhật tên mặt hàng
</commit_message>
<xml_diff>
--- a/Data_HDDT.xlsx
+++ b/Data_HDDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27131EF-5455-47EA-AD8B-7A4AD6554416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30302A1-21BB-4850-B28E-E7E4D7A0ABAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="271">
   <si>
     <t>Xăng RON 95-III</t>
   </si>
@@ -847,6 +847,9 @@
   </si>
   <si>
     <t>NoneNone</t>
+  </si>
+  <si>
+    <t>1K25TLD</t>
   </si>
 </sst>
 </file>
@@ -1338,7 +1341,7 @@
   <dimension ref="A2:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="9.9" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1867,7 +1870,7 @@
         <v>259</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Sửa lỗi bảng kê POS
</commit_message>
<xml_diff>
--- a/Data_HDDT.xlsx
+++ b/Data_HDDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30302A1-21BB-4850-B28E-E7E4D7A0ABAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B92FE21-7C15-4632-A7B0-9C0DD738572C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nhap lieu" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="271">
-  <si>
-    <t>Xăng RON 95-III</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="270">
   <si>
     <t>Mã kho</t>
   </si>
@@ -1341,1171 +1338,1172 @@
   <dimension ref="A2:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="9.9" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.44140625" style="1" customWidth="1"/>
-    <col min="10" max="390" width="8.44140625" style="1" customWidth="1"/>
-    <col min="391" max="16384" width="8.44140625" style="1"/>
+    <col min="2" max="3" width="9.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
+    <col min="10" max="390" width="8.42578125" style="1" customWidth="1"/>
+    <col min="391" max="16384" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>249</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+    </row>
+    <row r="8" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>246</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>247</v>
       </c>
       <c r="B10" s="6">
         <v>1000</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="I10" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B11" s="6">
         <v>1900</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="I11" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B12" s="6">
         <v>2000</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="I12" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="J12" s="6" t="s">
+      <c r="K12" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="K12" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="L12" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B13" s="6">
         <v>1000</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="I13" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="J13" s="6" t="s">
+      <c r="K13" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="L13" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="L13" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="I14" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="J14" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="J14" s="6" t="s">
+      <c r="K14" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="L14" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="L14" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="I15" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="D16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="I16" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="E17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="H20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="L20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="I21" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="L21" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
-        <v>108</v>
       </c>
       <c r="B22" s="1">
         <v>8</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="I22" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="E23" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J25" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="G25" s="4" t="s">
+      <c r="K25" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
         <v>129</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>130</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="I26" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="K26" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="I27" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
         <v>139</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>140</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="G28" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="I28" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="K28" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="L28" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" s="10">
         <v>131111</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="H29" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="K29" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="L29" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="10">
         <v>131112</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="G30" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="I30" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="K30" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="L30" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B31" s="10">
         <v>131114</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="G31" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="H31" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="J31" s="1" t="s">
+      <c r="K31" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="K31" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="L31" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="H32" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I32" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="J32" s="1" t="s">
+      <c r="K32" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="K32" s="2" t="s">
-        <v>173</v>
-      </c>
       <c r="L32" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" s="10">
         <v>51111</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G33" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="I33" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="10">
         <v>51115</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="F34" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="G34" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="G34" s="4" t="s">
-        <v>181</v>
-      </c>
       <c r="I34" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B35" s="10">
         <v>51112</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="F35" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="G35" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="I35" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="I35" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="K35" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="L35" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B36" s="10">
         <v>6321</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="F36" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="G36" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="I36" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
         <v>191</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>192</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="F37" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>196</v>
-      </c>
       <c r="I37" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B38" s="10">
         <v>333111</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="F38" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="G38" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="G38" s="4" t="s">
-        <v>200</v>
-      </c>
       <c r="I38" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="10">
         <v>333112</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="G39" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="G39" s="4" t="s">
-        <v>204</v>
-      </c>
       <c r="I39" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J39" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="K39" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>269</v>
-      </c>
       <c r="L39" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40" s="10">
         <v>333115</v>
@@ -2516,123 +2514,123 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
     </row>
-    <row r="42" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
     </row>
-    <row r="43" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
     </row>
-    <row r="44" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B44" s="10">
         <v>131111</v>
       </c>
       <c r="C44" s="10"/>
     </row>
-    <row r="45" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" s="10">
         <v>131112</v>
       </c>
       <c r="C45" s="10"/>
     </row>
-    <row r="46" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B46" s="10">
         <v>131114</v>
       </c>
       <c r="C46" s="10"/>
     </row>
-    <row r="47" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
     </row>
-    <row r="48" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" s="10">
         <v>3338111</v>
       </c>
       <c r="C48" s="10"/>
     </row>
-    <row r="49" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B49" s="10">
         <v>3338121</v>
       </c>
       <c r="C49" s="10"/>
     </row>
-    <row r="50" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B50" s="10">
         <v>333814</v>
       </c>
       <c r="C50" s="10"/>
     </row>
-    <row r="51" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B51" s="10">
         <v>6321</v>
       </c>
       <c r="C51" s="10"/>
     </row>
-    <row r="52" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
     </row>
-    <row r="53" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B53" s="10">
         <v>333111</v>
       </c>
       <c r="C53" s="10"/>
     </row>
-    <row r="54" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B54" s="10">
         <v>333112</v>
       </c>
       <c r="C54" s="10"/>
     </row>
-    <row r="55" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B55" s="10">
         <v>333115</v>

</xml_diff>

<commit_message>
Cập nhật Do 0.001 Nguyễn Huệ
</commit_message>
<xml_diff>
--- a/Data_HDDT.xlsx
+++ b/Data_HDDT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B92FE21-7C15-4632-A7B0-9C0DD738572C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F05A85C-7CEA-4046-AAAB-8430818950A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nhap lieu" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="272">
   <si>
     <t>Mã kho</t>
   </si>
@@ -847,6 +847,12 @@
   </si>
   <si>
     <t>1K25TLD</t>
+  </si>
+  <si>
+    <t>1K25TVP</t>
+  </si>
+  <si>
+    <t>HH050-022</t>
   </si>
 </sst>
 </file>
@@ -1338,24 +1344,24 @@
   <dimension ref="A2:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="9.9" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
-    <col min="10" max="390" width="8.42578125" style="1" customWidth="1"/>
-    <col min="391" max="16384" width="8.42578125" style="1"/>
+    <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
+    <col min="10" max="390" width="8.44140625" style="1" customWidth="1"/>
+    <col min="391" max="16384" width="8.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E2" s="1" t="s">
         <v>247</v>
       </c>
@@ -1381,14 +1387,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>247</v>
       </c>
@@ -1420,7 +1426,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>248</v>
       </c>
@@ -1452,7 +1458,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>246</v>
       </c>
@@ -1484,7 +1490,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>245</v>
       </c>
@@ -1519,7 +1525,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>31</v>
       </c>
@@ -1548,7 +1554,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
@@ -1577,7 +1583,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>246</v>
       </c>
@@ -1609,7 +1615,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>247</v>
       </c>
@@ -1641,7 +1647,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>248</v>
       </c>
@@ -1673,7 +1679,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>245</v>
       </c>
@@ -1705,7 +1711,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="5" t="s">
         <v>62</v>
       </c>
@@ -1734,7 +1740,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D15" s="4" t="s">
         <v>69</v>
       </c>
@@ -1763,7 +1769,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="D16" s="4" t="s">
         <v>74</v>
@@ -1790,7 +1796,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D17" s="4" t="s">
         <v>78</v>
       </c>
@@ -1819,7 +1825,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D18" s="4" t="s">
         <v>85</v>
       </c>
@@ -1845,7 +1851,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D19" s="4" t="s">
         <v>89</v>
       </c>
@@ -1874,7 +1880,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D20" s="4" t="s">
         <v>94</v>
       </c>
@@ -1903,7 +1909,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D21" s="4" t="s">
         <v>101</v>
       </c>
@@ -1929,7 +1935,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>107</v>
       </c>
@@ -1961,7 +1967,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D23" s="4" t="s">
         <v>112</v>
       </c>
@@ -1990,7 +1996,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
         <v>119</v>
       </c>
@@ -2016,7 +2022,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D25" s="4" t="s">
         <v>125</v>
       </c>
@@ -2042,7 +2048,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>129</v>
       </c>
@@ -2060,6 +2066,9 @@
       <c r="G26" s="4" t="s">
         <v>133</v>
       </c>
+      <c r="H26" s="1" t="s">
+        <v>271</v>
+      </c>
       <c r="I26" s="1" t="s">
         <v>236</v>
       </c>
@@ -2073,7 +2082,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -2102,7 +2111,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>139</v>
       </c>
@@ -2133,7 +2142,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>19</v>
       </c>
@@ -2169,7 +2178,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>36</v>
       </c>
@@ -2202,7 +2211,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>11</v>
       </c>
@@ -2238,7 +2247,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>242</v>
       </c>
@@ -2272,7 +2281,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>19</v>
       </c>
@@ -2305,7 +2314,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>36</v>
       </c>
@@ -2338,7 +2347,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>11</v>
       </c>
@@ -2371,7 +2380,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>243</v>
       </c>
@@ -2404,7 +2413,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>191</v>
       </c>
@@ -2435,7 +2444,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>19</v>
       </c>
@@ -2462,13 +2471,13 @@
         <v>266</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>36</v>
       </c>
@@ -2501,7 +2510,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>11</v>
       </c>
@@ -2514,26 +2523,26 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
     </row>
-    <row r="42" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>204</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
     </row>
-    <row r="43" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>139</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
     </row>
-    <row r="44" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>19</v>
       </c>
@@ -2542,7 +2551,7 @@
       </c>
       <c r="C44" s="10"/>
     </row>
-    <row r="45" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>36</v>
       </c>
@@ -2551,7 +2560,7 @@
       </c>
       <c r="C45" s="10"/>
     </row>
-    <row r="46" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>11</v>
       </c>
@@ -2560,14 +2569,14 @@
       </c>
       <c r="C46" s="10"/>
     </row>
-    <row r="47" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>244</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
     </row>
-    <row r="48" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>19</v>
       </c>
@@ -2576,7 +2585,7 @@
       </c>
       <c r="C48" s="10"/>
     </row>
-    <row r="49" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>36</v>
       </c>
@@ -2585,7 +2594,7 @@
       </c>
       <c r="C49" s="10"/>
     </row>
-    <row r="50" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>11</v>
       </c>
@@ -2594,7 +2603,7 @@
       </c>
       <c r="C50" s="10"/>
     </row>
-    <row r="51" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>243</v>
       </c>
@@ -2603,14 +2612,14 @@
       </c>
       <c r="C51" s="10"/>
     </row>
-    <row r="52" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>191</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
     </row>
-    <row r="53" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>19</v>
       </c>
@@ -2619,7 +2628,7 @@
       </c>
       <c r="C53" s="10"/>
     </row>
-    <row r="54" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>36</v>
       </c>
@@ -2628,7 +2637,7 @@
       </c>
       <c r="C54" s="10"/>
     </row>
-    <row r="55" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Cập nhật thêm cột số cửa hàng
</commit_message>
<xml_diff>
--- a/Data_HDDT.xlsx
+++ b/Data_HDDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F05A85C-7CEA-4046-AAAB-8430818950A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570F209F-2D29-47C9-801A-ADC0B63F8B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nhap lieu" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="278">
   <si>
     <t>Mã kho</t>
   </si>
@@ -853,6 +853,24 @@
   </si>
   <si>
     <t>HH050-022</t>
+  </si>
+  <si>
+    <t>1K25TBX</t>
+  </si>
+  <si>
+    <t>1K25TAT</t>
+  </si>
+  <si>
+    <t>1K25TML</t>
+  </si>
+  <si>
+    <t>1K25TNC</t>
+  </si>
+  <si>
+    <t>1K25TTP</t>
+  </si>
+  <si>
+    <t>1K25TXT</t>
   </si>
 </sst>
 </file>
@@ -1343,25 +1361,25 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="9.9" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
-    <col min="10" max="390" width="8.44140625" style="1" customWidth="1"/>
-    <col min="391" max="16384" width="8.44140625" style="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
+    <col min="10" max="390" width="8.42578125" style="1" customWidth="1"/>
+    <col min="391" max="16384" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="1" t="s">
         <v>247</v>
       </c>
@@ -1387,14 +1405,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>247</v>
       </c>
@@ -1420,13 +1438,13 @@
         <v>249</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>248</v>
       </c>
@@ -1458,7 +1476,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>246</v>
       </c>
@@ -1490,7 +1508,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>245</v>
       </c>
@@ -1525,7 +1543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="4" t="s">
         <v>31</v>
       </c>
@@ -1554,7 +1572,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
@@ -1583,7 +1601,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>246</v>
       </c>
@@ -1615,7 +1633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>247</v>
       </c>
@@ -1647,7 +1665,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>248</v>
       </c>
@@ -1679,7 +1697,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>245</v>
       </c>
@@ -1711,7 +1729,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
         <v>62</v>
       </c>
@@ -1740,7 +1758,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="4" t="s">
         <v>69</v>
       </c>
@@ -1769,7 +1787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="D16" s="4" t="s">
         <v>74</v>
@@ -1796,7 +1814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="4" t="s">
         <v>78</v>
       </c>
@@ -1825,7 +1843,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="4" t="s">
         <v>85</v>
       </c>
@@ -1851,7 +1869,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" s="4" t="s">
         <v>89</v>
       </c>
@@ -1880,7 +1898,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D20" s="4" t="s">
         <v>94</v>
       </c>
@@ -1909,7 +1927,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="4" t="s">
         <v>101</v>
       </c>
@@ -1935,7 +1953,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>107</v>
       </c>
@@ -1961,13 +1979,13 @@
         <v>259</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" s="4" t="s">
         <v>112</v>
       </c>
@@ -1996,7 +2014,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="4" t="s">
         <v>119</v>
       </c>
@@ -2022,7 +2040,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="4" t="s">
         <v>125</v>
       </c>
@@ -2048,7 +2066,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>129</v>
       </c>
@@ -2082,7 +2100,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -2105,13 +2123,13 @@
         <v>261</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>139</v>
       </c>
@@ -2142,7 +2160,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>19</v>
       </c>
@@ -2178,7 +2196,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>36</v>
       </c>
@@ -2211,7 +2229,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>11</v>
       </c>
@@ -2247,7 +2265,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>242</v>
       </c>
@@ -2281,7 +2299,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>19</v>
       </c>
@@ -2308,13 +2326,13 @@
         <v>262</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>36</v>
       </c>
@@ -2341,13 +2359,13 @@
         <v>263</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>11</v>
       </c>
@@ -2380,7 +2398,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>243</v>
       </c>
@@ -2413,7 +2431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>191</v>
       </c>
@@ -2444,7 +2462,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
         <v>19</v>
       </c>
@@ -2477,7 +2495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>36</v>
       </c>
@@ -2504,13 +2522,13 @@
         <v>267</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>11</v>
       </c>
@@ -2523,26 +2541,26 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
     </row>
-    <row r="42" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>204</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
     </row>
-    <row r="43" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>139</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
     </row>
-    <row r="44" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>19</v>
       </c>
@@ -2551,7 +2569,7 @@
       </c>
       <c r="C44" s="10"/>
     </row>
-    <row r="45" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>36</v>
       </c>
@@ -2560,7 +2578,7 @@
       </c>
       <c r="C45" s="10"/>
     </row>
-    <row r="46" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>11</v>
       </c>
@@ -2569,14 +2587,14 @@
       </c>
       <c r="C46" s="10"/>
     </row>
-    <row r="47" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>244</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
     </row>
-    <row r="48" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>19</v>
       </c>
@@ -2585,7 +2603,7 @@
       </c>
       <c r="C48" s="10"/>
     </row>
-    <row r="49" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>36</v>
       </c>
@@ -2594,7 +2612,7 @@
       </c>
       <c r="C49" s="10"/>
     </row>
-    <row r="50" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
         <v>11</v>
       </c>
@@ -2603,7 +2621,7 @@
       </c>
       <c r="C50" s="10"/>
     </row>
-    <row r="51" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
         <v>243</v>
       </c>
@@ -2612,14 +2630,14 @@
       </c>
       <c r="C51" s="10"/>
     </row>
-    <row r="52" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>191</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
     </row>
-    <row r="53" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
         <v>19</v>
       </c>
@@ -2628,7 +2646,7 @@
       </c>
       <c r="C53" s="10"/>
     </row>
-    <row r="54" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>36</v>
       </c>
@@ -2637,7 +2655,7 @@
       </c>
       <c r="C54" s="10"/>
     </row>
-    <row r="55" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Cập nhật logic dat ten file
</commit_message>
<xml_diff>
--- a/Data_HDDT.xlsx
+++ b/Data_HDDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570F209F-2D29-47C9-801A-ADC0B63F8B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8EED60-1B8C-49C7-894A-EA5D4A712E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nhap lieu" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="279">
   <si>
     <t>Mã kho</t>
   </si>
@@ -871,6 +871,9 @@
   </si>
   <si>
     <t>1K25TXT</t>
+  </si>
+  <si>
+    <t>1K25TTS</t>
   </si>
 </sst>
 </file>
@@ -1361,25 +1364,25 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="9.9" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
-    <col min="10" max="390" width="8.42578125" style="1" customWidth="1"/>
-    <col min="391" max="16384" width="8.42578125" style="1"/>
+    <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
+    <col min="10" max="390" width="8.44140625" style="1" customWidth="1"/>
+    <col min="391" max="16384" width="8.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E2" s="1" t="s">
         <v>247</v>
       </c>
@@ -1405,14 +1408,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>247</v>
       </c>
@@ -1444,7 +1447,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>248</v>
       </c>
@@ -1476,7 +1479,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>246</v>
       </c>
@@ -1508,7 +1511,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>245</v>
       </c>
@@ -1543,7 +1546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>31</v>
       </c>
@@ -1566,13 +1569,13 @@
         <v>251</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
@@ -1601,7 +1604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>246</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>247</v>
       </c>
@@ -1665,7 +1668,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>248</v>
       </c>
@@ -1697,7 +1700,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>245</v>
       </c>
@@ -1729,7 +1732,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="5" t="s">
         <v>62</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D15" s="4" t="s">
         <v>69</v>
       </c>
@@ -1787,7 +1790,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="D16" s="4" t="s">
         <v>74</v>
@@ -1814,7 +1817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D17" s="4" t="s">
         <v>78</v>
       </c>
@@ -1843,7 +1846,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D18" s="4" t="s">
         <v>85</v>
       </c>
@@ -1869,7 +1872,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D19" s="4" t="s">
         <v>89</v>
       </c>
@@ -1898,7 +1901,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D20" s="4" t="s">
         <v>94</v>
       </c>
@@ -1927,7 +1930,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D21" s="4" t="s">
         <v>101</v>
       </c>
@@ -1953,7 +1956,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>107</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D23" s="4" t="s">
         <v>112</v>
       </c>
@@ -2014,7 +2017,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
         <v>119</v>
       </c>
@@ -2040,7 +2043,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D25" s="4" t="s">
         <v>125</v>
       </c>
@@ -2066,7 +2069,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>129</v>
       </c>
@@ -2100,7 +2103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -2129,7 +2132,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>139</v>
       </c>
@@ -2160,7 +2163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>19</v>
       </c>
@@ -2196,7 +2199,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>36</v>
       </c>
@@ -2229,7 +2232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>11</v>
       </c>
@@ -2265,7 +2268,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>242</v>
       </c>
@@ -2299,7 +2302,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>19</v>
       </c>
@@ -2332,7 +2335,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>36</v>
       </c>
@@ -2365,7 +2368,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>11</v>
       </c>
@@ -2398,7 +2401,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>243</v>
       </c>
@@ -2431,7 +2434,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>191</v>
       </c>
@@ -2462,7 +2465,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>19</v>
       </c>
@@ -2495,7 +2498,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>36</v>
       </c>
@@ -2528,7 +2531,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>11</v>
       </c>
@@ -2541,26 +2544,26 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
     </row>
-    <row r="42" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>204</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
     </row>
-    <row r="43" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>139</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
     </row>
-    <row r="44" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>19</v>
       </c>
@@ -2569,7 +2572,7 @@
       </c>
       <c r="C44" s="10"/>
     </row>
-    <row r="45" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>36</v>
       </c>
@@ -2578,7 +2581,7 @@
       </c>
       <c r="C45" s="10"/>
     </row>
-    <row r="46" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>11</v>
       </c>
@@ -2587,14 +2590,14 @@
       </c>
       <c r="C46" s="10"/>
     </row>
-    <row r="47" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>244</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
     </row>
-    <row r="48" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>19</v>
       </c>
@@ -2603,7 +2606,7 @@
       </c>
       <c r="C48" s="10"/>
     </row>
-    <row r="49" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>36</v>
       </c>
@@ -2612,7 +2615,7 @@
       </c>
       <c r="C49" s="10"/>
     </row>
-    <row r="50" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>11</v>
       </c>
@@ -2621,7 +2624,7 @@
       </c>
       <c r="C50" s="10"/>
     </row>
-    <row r="51" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>243</v>
       </c>
@@ -2630,14 +2633,14 @@
       </c>
       <c r="C51" s="10"/>
     </row>
-    <row r="52" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>191</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
     </row>
-    <row r="53" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>19</v>
       </c>
@@ -2646,7 +2649,7 @@
       </c>
       <c r="C53" s="10"/>
     </row>
-    <row r="54" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>36</v>
       </c>
@@ -2655,7 +2658,7 @@
       </c>
       <c r="C54" s="10"/>
     </row>
-    <row r="55" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Cập nhật theo cấu trúc file hddt mới
</commit_message>
<xml_diff>
--- a/Data_HDDT.xlsx
+++ b/Data_HDDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8EED60-1B8C-49C7-894A-EA5D4A712E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DCD15E-AEBD-49C0-9F4F-DF5699D9253A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="287">
   <si>
     <t>Mã kho</t>
   </si>
@@ -843,9 +843,6 @@
     <t>KDNL017</t>
   </si>
   <si>
-    <t>NoneNone</t>
-  </si>
-  <si>
     <t>1K25TLD</t>
   </si>
   <si>
@@ -874,6 +871,33 @@
   </si>
   <si>
     <t>1K25TTS</t>
+  </si>
+  <si>
+    <t>1K25TCT</t>
+  </si>
+  <si>
+    <t>1K25TGT</t>
+  </si>
+  <si>
+    <t>1K25TGX</t>
+  </si>
+  <si>
+    <t>1K25TKH</t>
+  </si>
+  <si>
+    <t>1K25TDT</t>
+  </si>
+  <si>
+    <t>1K25TLM</t>
+  </si>
+  <si>
+    <t>1K25TNV</t>
+  </si>
+  <si>
+    <t>1K25TTA</t>
+  </si>
+  <si>
+    <t>1K25TTR</t>
   </si>
 </sst>
 </file>
@@ -1364,8 +1388,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="9.9" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1441,7 +1465,7 @@
         <v>249</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>11</v>
@@ -1472,7 +1496,7 @@
       <c r="J5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -1504,7 +1528,7 @@
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L6" s="1" t="s">
@@ -1540,7 +1564,7 @@
         <v>250</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>11</v>
@@ -1569,7 +1593,7 @@
         <v>251</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>36</v>
@@ -1598,7 +1622,7 @@
         <v>252</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>11</v>
@@ -1630,7 +1654,7 @@
         <v>253</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>11</v>
@@ -1661,8 +1685,8 @@
       <c r="J11" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>268</v>
+      <c r="K11" s="6" t="s">
+        <v>279</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>19</v>
@@ -1693,7 +1717,7 @@
       <c r="J12" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="6" t="s">
         <v>55</v>
       </c>
       <c r="L12" s="6" t="s">
@@ -1725,7 +1749,7 @@
       <c r="J13" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="6" t="s">
         <v>61</v>
       </c>
       <c r="L13" s="6" t="s">
@@ -1754,7 +1778,7 @@
       <c r="J14" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="6" t="s">
         <v>68</v>
       </c>
       <c r="L14" s="6" t="s">
@@ -1784,7 +1808,7 @@
         <v>255</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>11</v>
@@ -1811,7 +1835,7 @@
         <v>256</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>11</v>
@@ -1839,7 +1863,7 @@
       <c r="J17" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="1" t="s">
         <v>84</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -1866,7 +1890,7 @@
         <v>257</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>19</v>
@@ -1894,8 +1918,8 @@
       <c r="J19" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>269</v>
+      <c r="K19" s="1" t="s">
+        <v>268</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>19</v>
@@ -1923,7 +1947,7 @@
       <c r="J20" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K20" s="1" t="s">
         <v>100</v>
       </c>
       <c r="L20" s="1" t="s">
@@ -1949,7 +1973,7 @@
       <c r="J21" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L21" s="1" t="s">
@@ -1982,7 +2006,7 @@
         <v>259</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>19</v>
@@ -2010,7 +2034,7 @@
       <c r="J23" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="K23" s="1" t="s">
         <v>118</v>
       </c>
       <c r="L23" s="1" t="s">
@@ -2036,7 +2060,7 @@
       <c r="J24" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="K24" s="1" t="s">
         <v>124</v>
       </c>
       <c r="L24" s="1" t="s">
@@ -2063,7 +2087,7 @@
         <v>260</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>19</v>
@@ -2088,7 +2112,7 @@
         <v>133</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>236</v>
@@ -2126,7 +2150,7 @@
         <v>261</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>36</v>
@@ -2156,7 +2180,7 @@
       <c r="J28" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="K28" s="1" t="s">
         <v>145</v>
       </c>
       <c r="L28" s="1" t="s">
@@ -2192,7 +2216,7 @@
       <c r="J29" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="K29" s="1" t="s">
         <v>152</v>
       </c>
       <c r="L29" s="1" t="s">
@@ -2225,7 +2249,7 @@
       <c r="J30" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="K30" s="1" t="s">
         <v>158</v>
       </c>
       <c r="L30" s="1" t="s">
@@ -2261,7 +2285,7 @@
       <c r="J31" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="K31" s="1" t="s">
         <v>165</v>
       </c>
       <c r="L31" s="1" t="s">
@@ -2295,7 +2319,7 @@
       <c r="J32" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="K32" s="1" t="s">
         <v>172</v>
       </c>
       <c r="L32" s="1" t="s">
@@ -2329,7 +2353,7 @@
         <v>262</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>11</v>
@@ -2362,7 +2386,7 @@
         <v>263</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>36</v>
@@ -2394,7 +2418,7 @@
       <c r="J35" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="K35" s="1" t="s">
         <v>186</v>
       </c>
       <c r="L35" s="1" t="s">
@@ -2428,7 +2452,7 @@
         <v>264</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>268</v>
+        <v>285</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>11</v>
@@ -2459,7 +2483,7 @@
         <v>265</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>11</v>
@@ -2492,7 +2516,7 @@
         <v>266</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>11</v>
@@ -2525,7 +2549,7 @@
         <v>267</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Cập nhật dải hd các CHXD chi nhanh
</commit_message>
<xml_diff>
--- a/Data_HDDT.xlsx
+++ b/Data_HDDT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DCD15E-AEBD-49C0-9F4F-DF5699D9253A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E940768D-3441-4173-8FB5-E4FE4AEE7152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nhap lieu" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="289">
   <si>
     <t>Mã kho</t>
   </si>
@@ -219,12 +219,6 @@
     <t>HH009HS</t>
   </si>
   <si>
-    <t>KDNL007</t>
-  </si>
-  <si>
-    <t>1K25TDP</t>
-  </si>
-  <si>
     <t>Hùng Vương</t>
   </si>
   <si>
@@ -288,9 +282,6 @@
     <t>HH050-8</t>
   </si>
   <si>
-    <t>KDNL019</t>
-  </si>
-  <si>
     <t>1K25TLP</t>
   </si>
   <si>
@@ -441,9 +432,6 @@
     <t>HH009B</t>
   </si>
   <si>
-    <t>KDNL057</t>
-  </si>
-  <si>
     <t>Nhân Chính</t>
   </si>
   <si>
@@ -471,9 +459,6 @@
     <t>HH009NG</t>
   </si>
   <si>
-    <t>KDNL062</t>
-  </si>
-  <si>
     <t>1K25TNG</t>
   </si>
   <si>
@@ -492,9 +477,6 @@
     <t>HH050-9</t>
   </si>
   <si>
-    <t>KDNL054</t>
-  </si>
-  <si>
     <t>1K25TPL</t>
   </si>
   <si>
@@ -510,9 +492,6 @@
     <t>HH009007</t>
   </si>
   <si>
-    <t>KDNL068</t>
-  </si>
-  <si>
     <t>1K25TQT</t>
   </si>
   <si>
@@ -552,9 +531,6 @@
     <t>HH050-10</t>
   </si>
   <si>
-    <t>KDNL060</t>
-  </si>
-  <si>
     <t>1K25TTD</t>
   </si>
   <si>
@@ -786,30 +762,9 @@
     <t>Xăng RON95 Mức 3</t>
   </si>
   <si>
-    <t>KDNL072</t>
-  </si>
-  <si>
-    <t>KDNL070</t>
-  </si>
-  <si>
-    <t>KDNL076</t>
-  </si>
-  <si>
-    <t>KDNL059</t>
-  </si>
-  <si>
-    <t>KDNL074</t>
-  </si>
-  <si>
     <t>KDNL011</t>
   </si>
   <si>
-    <t>KDNL009</t>
-  </si>
-  <si>
-    <t>KDNL058</t>
-  </si>
-  <si>
     <t>KDNL002</t>
   </si>
   <si>
@@ -822,24 +777,6 @@
     <t>KDNL015</t>
   </si>
   <si>
-    <t>KDNL056</t>
-  </si>
-  <si>
-    <t>KDNL071</t>
-  </si>
-  <si>
-    <t>KDNL055</t>
-  </si>
-  <si>
-    <t>KDNL067</t>
-  </si>
-  <si>
-    <t>KDNL073</t>
-  </si>
-  <si>
-    <t>KDNL075</t>
-  </si>
-  <si>
     <t>KDNL017</t>
   </si>
   <si>
@@ -855,9 +792,6 @@
     <t>1K25TBX</t>
   </si>
   <si>
-    <t>1K25TAT</t>
-  </si>
-  <si>
     <t>1K25TML</t>
   </si>
   <si>
@@ -873,21 +807,12 @@
     <t>1K25TTS</t>
   </si>
   <si>
-    <t>1K25TCT</t>
-  </si>
-  <si>
     <t>1K25TGT</t>
   </si>
   <si>
     <t>1K25TGX</t>
   </si>
   <si>
-    <t>1K25TKH</t>
-  </si>
-  <si>
-    <t>1K25TDT</t>
-  </si>
-  <si>
     <t>1K25TLM</t>
   </si>
   <si>
@@ -898,6 +823,87 @@
   </si>
   <si>
     <t>1K25TTR</t>
+  </si>
+  <si>
+    <t>KDNL172</t>
+  </si>
+  <si>
+    <t>KDNL170</t>
+  </si>
+  <si>
+    <t>1K25TNP</t>
+  </si>
+  <si>
+    <t>KDNL176</t>
+  </si>
+  <si>
+    <t>KDNL159</t>
+  </si>
+  <si>
+    <t>1K25TAB</t>
+  </si>
+  <si>
+    <t>KDNL174</t>
+  </si>
+  <si>
+    <t>KDNL107</t>
+  </si>
+  <si>
+    <t>1K25THS</t>
+  </si>
+  <si>
+    <t>KDNL109</t>
+  </si>
+  <si>
+    <t>1K25TAC</t>
+  </si>
+  <si>
+    <t>KDNL158</t>
+  </si>
+  <si>
+    <t>1K25TKN</t>
+  </si>
+  <si>
+    <t>KDNL119</t>
+  </si>
+  <si>
+    <t>KDNL157</t>
+  </si>
+  <si>
+    <t>1K25TAA</t>
+  </si>
+  <si>
+    <t>KDNL156</t>
+  </si>
+  <si>
+    <t>KDNL162</t>
+  </si>
+  <si>
+    <t>KDNL154</t>
+  </si>
+  <si>
+    <t>KDNL168</t>
+  </si>
+  <si>
+    <t>KDNL160</t>
+  </si>
+  <si>
+    <t>KDNL171</t>
+  </si>
+  <si>
+    <t>1K25TTT</t>
+  </si>
+  <si>
+    <t>KDNL155</t>
+  </si>
+  <si>
+    <t>KDNL167</t>
+  </si>
+  <si>
+    <t>KDNL173</t>
+  </si>
+  <si>
+    <t>KDNL175</t>
   </si>
 </sst>
 </file>
@@ -1389,38 +1395,38 @@
   <dimension ref="A2:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="9.9" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
-    <col min="10" max="390" width="8.44140625" style="1" customWidth="1"/>
-    <col min="391" max="16384" width="8.44140625" style="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
+    <col min="10" max="390" width="8.42578125" style="1" customWidth="1"/>
+    <col min="391" max="16384" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>0</v>
@@ -1432,16 +1438,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1459,21 +1465,21 @@
         <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -1491,7 +1497,7 @@
         <v>16</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>17</v>
@@ -1503,9 +1509,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -1523,7 +1529,7 @@
         <v>22</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>23</v>
@@ -1535,9 +1541,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>25</v>
@@ -1558,19 +1564,19 @@
         <v>30</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="4" t="s">
         <v>31</v>
       </c>
@@ -1587,19 +1593,19 @@
         <v>35</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>277</v>
+        <v>255</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
@@ -1616,21 +1622,21 @@
         <v>41</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B10" s="6">
         <v>1000</v>
@@ -1648,21 +1654,21 @@
         <v>45</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B11" s="6">
         <v>1900</v>
@@ -1680,21 +1686,21 @@
         <v>49</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B12" s="6">
         <v>2000</v>
@@ -1712,7 +1718,7 @@
         <v>53</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>54</v>
@@ -1720,13 +1726,13 @@
       <c r="K12" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="L12" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B13" s="6">
         <v>1000</v>
@@ -1744,450 +1750,450 @@
         <v>59</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="J13" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="5" t="s">
+      <c r="J14" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="K14" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="J14" s="6" t="s">
+      <c r="L14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="L14" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="H15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="I15" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="D16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="I16" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="H17" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="I17" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="L17" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="E18" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="F18" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="I18" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="H19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="I19" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="F20" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="H20" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="I20" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="K20" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="L20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="E21" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="F21" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="I21" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="K21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="L21" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="B22" s="1">
         <v>8</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="I22" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="G23" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="L25" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
         <v>126</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>129</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>133</v>
-      </c>
       <c r="H26" s="1" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>134</v>
+        <v>276</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>124</v>
+        <v>277</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
         <v>135</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>139</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="K28" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="L28" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>19</v>
       </c>
@@ -2196,34 +2202,34 @@
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="L29" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>36</v>
       </c>
@@ -2232,31 +2238,31 @@
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>157</v>
+        <v>281</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>11</v>
       </c>
@@ -2265,68 +2271,68 @@
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>19</v>
       </c>
@@ -2335,31 +2341,31 @@
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="4" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>262</v>
+        <v>283</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>36</v>
       </c>
@@ -2368,31 +2374,31 @@
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="4" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>263</v>
+        <v>285</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>275</v>
+        <v>253</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>11</v>
       </c>
@@ -2401,95 +2407,95 @@
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="4" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B36" s="10">
         <v>6321</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="4" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="4" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>265</v>
+        <v>287</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
         <v>19</v>
       </c>
@@ -2498,31 +2504,31 @@
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="4" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>266</v>
+        <v>288</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>36</v>
       </c>
@@ -2531,31 +2537,31 @@
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="4" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>11</v>
       </c>
@@ -2568,26 +2574,26 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
     </row>
-    <row r="42" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
     </row>
-    <row r="43" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
     </row>
-    <row r="44" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>19</v>
       </c>
@@ -2596,7 +2602,7 @@
       </c>
       <c r="C44" s="10"/>
     </row>
-    <row r="45" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>36</v>
       </c>
@@ -2605,7 +2611,7 @@
       </c>
       <c r="C45" s="10"/>
     </row>
-    <row r="46" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>11</v>
       </c>
@@ -2614,14 +2620,14 @@
       </c>
       <c r="C46" s="10"/>
     </row>
-    <row r="47" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
     </row>
-    <row r="48" spans="1:12" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>19</v>
       </c>
@@ -2630,7 +2636,7 @@
       </c>
       <c r="C48" s="10"/>
     </row>
-    <row r="49" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>36</v>
       </c>
@@ -2639,7 +2645,7 @@
       </c>
       <c r="C49" s="10"/>
     </row>
-    <row r="50" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
         <v>11</v>
       </c>
@@ -2648,23 +2654,23 @@
       </c>
       <c r="C50" s="10"/>
     </row>
-    <row r="51" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B51" s="10">
         <v>6321</v>
       </c>
       <c r="C51" s="10"/>
     </row>
-    <row r="52" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
     </row>
-    <row r="53" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
         <v>19</v>
       </c>
@@ -2673,7 +2679,7 @@
       </c>
       <c r="C53" s="10"/>
     </row>
-    <row r="54" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>36</v>
       </c>
@@ -2682,7 +2688,7 @@
       </c>
       <c r="C54" s="10"/>
     </row>
-    <row r="55" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Cập nhật mã kho mã khách
</commit_message>
<xml_diff>
--- a/Data_HDDT.xlsx
+++ b/Data_HDDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E940768D-3441-4173-8FB5-E4FE4AEE7152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E4028E8-A79E-48CA-8FFB-1B074B1F8EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="320">
   <si>
     <t>Mã kho</t>
   </si>
@@ -904,6 +904,99 @@
   </si>
   <si>
     <t>KDNL175</t>
+  </si>
+  <si>
+    <t>Mã khách</t>
+  </si>
+  <si>
+    <t>KDNL072</t>
+  </si>
+  <si>
+    <t>KDNL070</t>
+  </si>
+  <si>
+    <t>KDNL076</t>
+  </si>
+  <si>
+    <t>KDNL059</t>
+  </si>
+  <si>
+    <t>KDNL074</t>
+  </si>
+  <si>
+    <t>KDNL007</t>
+  </si>
+  <si>
+    <t>KDNL009</t>
+  </si>
+  <si>
+    <t>KDNL058</t>
+  </si>
+  <si>
+    <t>KDNL019</t>
+  </si>
+  <si>
+    <t>KDNL057</t>
+  </si>
+  <si>
+    <t>KDNL056</t>
+  </si>
+  <si>
+    <t>KDNL062</t>
+  </si>
+  <si>
+    <t>KDNL054</t>
+  </si>
+  <si>
+    <t>KDNL068</t>
+  </si>
+  <si>
+    <t>KDNL060</t>
+  </si>
+  <si>
+    <t>KDNL071</t>
+  </si>
+  <si>
+    <t>KDNL055</t>
+  </si>
+  <si>
+    <t>KDNL067</t>
+  </si>
+  <si>
+    <t>KDNL073</t>
+  </si>
+  <si>
+    <t>KDNL075</t>
+  </si>
+  <si>
+    <t>TN0000</t>
+  </si>
+  <si>
+    <t>HH050-028</t>
+  </si>
+  <si>
+    <t>HH050-025</t>
+  </si>
+  <si>
+    <t>HH050-027</t>
+  </si>
+  <si>
+    <t>HH050-023</t>
+  </si>
+  <si>
+    <t>HH050-024</t>
+  </si>
+  <si>
+    <t>HH050-14</t>
+  </si>
+  <si>
+    <t>HH050-020</t>
+  </si>
+  <si>
+    <t>HH050-029</t>
+  </si>
+  <si>
+    <t>HH050-19</t>
   </si>
 </sst>
 </file>
@@ -1392,10 +1485,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:L55"/>
+  <dimension ref="A2:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1412,7 +1505,7 @@
     <col min="391" max="16384" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="1" t="s">
         <v>239</v>
       </c>
@@ -1437,15 +1530,18 @@
       <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>239</v>
       </c>
@@ -1464,6 +1560,9 @@
       <c r="G4" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>319</v>
+      </c>
       <c r="I4" s="1" t="s">
         <v>198</v>
       </c>
@@ -1476,8 +1575,11 @@
       <c r="L4" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>240</v>
       </c>
@@ -1508,8 +1610,11 @@
       <c r="L5" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>238</v>
       </c>
@@ -1540,8 +1645,11 @@
       <c r="L6" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>237</v>
       </c>
@@ -1575,8 +1683,11 @@
       <c r="L7" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="4" t="s">
         <v>31</v>
       </c>
@@ -1604,8 +1715,11 @@
       <c r="L8" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
@@ -1621,6 +1735,9 @@
       <c r="G9" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="H9" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="I9" s="1" t="s">
         <v>222</v>
       </c>
@@ -1633,8 +1750,11 @@
       <c r="L9" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>238</v>
       </c>
@@ -1665,8 +1785,11 @@
       <c r="L10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>239</v>
       </c>
@@ -1697,8 +1820,11 @@
       <c r="L11" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>240</v>
       </c>
@@ -1729,8 +1855,11 @@
       <c r="L12" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>237</v>
       </c>
@@ -1761,8 +1890,11 @@
       <c r="L13" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
         <v>60</v>
       </c>
@@ -1790,8 +1922,11 @@
       <c r="L14" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="4" t="s">
         <v>67</v>
       </c>
@@ -1819,8 +1954,11 @@
       <c r="L15" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M15" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="D16" s="4" t="s">
         <v>72</v>
@@ -1846,8 +1984,11 @@
       <c r="L16" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M16" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="4" t="s">
         <v>76</v>
       </c>
@@ -1875,8 +2016,11 @@
       <c r="L17" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M17" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="4" t="s">
         <v>82</v>
       </c>
@@ -1889,6 +2033,9 @@
       <c r="G18" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="H18" s="1" t="s">
+        <v>312</v>
+      </c>
       <c r="I18" s="1" t="s">
         <v>204</v>
       </c>
@@ -1901,8 +2048,11 @@
       <c r="L18" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M18" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" s="4" t="s">
         <v>86</v>
       </c>
@@ -1930,8 +2080,11 @@
       <c r="L19" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M19" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D20" s="4" t="s">
         <v>91</v>
       </c>
@@ -1959,8 +2112,11 @@
       <c r="L20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M20" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="4" t="s">
         <v>98</v>
       </c>
@@ -1973,6 +2129,9 @@
       <c r="G21" s="4" t="s">
         <v>101</v>
       </c>
+      <c r="H21" s="1" t="s">
+        <v>315</v>
+      </c>
       <c r="I21" s="1" t="s">
         <v>206</v>
       </c>
@@ -1985,8 +2144,11 @@
       <c r="L21" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M21" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>104</v>
       </c>
@@ -2005,6 +2167,9 @@
       <c r="G22" s="4" t="s">
         <v>108</v>
       </c>
+      <c r="H22" s="1" t="s">
+        <v>313</v>
+      </c>
       <c r="I22" s="1" t="s">
         <v>203</v>
       </c>
@@ -2017,8 +2182,11 @@
       <c r="L22" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M22" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" s="4" t="s">
         <v>109</v>
       </c>
@@ -2046,8 +2214,11 @@
       <c r="L23" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M23" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="4" t="s">
         <v>116</v>
       </c>
@@ -2060,6 +2231,9 @@
       <c r="G24" s="4" t="s">
         <v>119</v>
       </c>
+      <c r="H24" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="I24" s="1" t="s">
         <v>214</v>
       </c>
@@ -2072,8 +2246,11 @@
       <c r="L24" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M24" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="4" t="s">
         <v>122</v>
       </c>
@@ -2086,6 +2263,9 @@
       <c r="G25" s="4" t="s">
         <v>125</v>
       </c>
+      <c r="H25" s="4" t="s">
+        <v>311</v>
+      </c>
       <c r="I25" s="1" t="s">
         <v>213</v>
       </c>
@@ -2098,8 +2278,11 @@
       <c r="L25" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M25" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>126</v>
       </c>
@@ -2132,8 +2315,11 @@
       <c r="L26" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M26" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -2161,8 +2347,11 @@
       <c r="L27" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M27" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>135</v>
       </c>
@@ -2192,8 +2381,11 @@
       <c r="L28" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M28" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>19</v>
       </c>
@@ -2228,8 +2420,11 @@
       <c r="L29" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M29" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>36</v>
       </c>
@@ -2261,8 +2456,11 @@
       <c r="L30" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M30" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>11</v>
       </c>
@@ -2297,8 +2495,11 @@
       <c r="L31" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M31" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>234</v>
       </c>
@@ -2331,8 +2532,11 @@
       <c r="L32" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M32" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>19</v>
       </c>
@@ -2364,8 +2568,11 @@
       <c r="L33" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M33" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>36</v>
       </c>
@@ -2397,8 +2604,11 @@
       <c r="L34" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M34" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>11</v>
       </c>
@@ -2430,8 +2640,11 @@
       <c r="L35" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M35" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>235</v>
       </c>
@@ -2463,8 +2676,11 @@
       <c r="L36" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M36" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>183</v>
       </c>
@@ -2482,6 +2698,9 @@
       <c r="G37" s="4" t="s">
         <v>187</v>
       </c>
+      <c r="H37" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="I37" s="1" t="s">
         <v>199</v>
       </c>
@@ -2494,8 +2713,11 @@
       <c r="L37" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M37" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
         <v>19</v>
       </c>
@@ -2527,8 +2749,11 @@
       <c r="L38" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M38" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>36</v>
       </c>
@@ -2548,6 +2773,9 @@
       <c r="G39" s="4" t="s">
         <v>195</v>
       </c>
+      <c r="H39" s="1" t="s">
+        <v>317</v>
+      </c>
       <c r="I39" s="1" t="s">
         <v>216</v>
       </c>
@@ -2560,8 +2788,11 @@
       <c r="L39" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M39" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>11</v>
       </c>
@@ -2574,26 +2805,26 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
     </row>
-    <row r="42" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>196</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
     </row>
-    <row r="43" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>135</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
     </row>
-    <row r="44" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>19</v>
       </c>
@@ -2602,7 +2833,7 @@
       </c>
       <c r="C44" s="10"/>
     </row>
-    <row r="45" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>36</v>
       </c>
@@ -2611,7 +2842,7 @@
       </c>
       <c r="C45" s="10"/>
     </row>
-    <row r="46" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>11</v>
       </c>
@@ -2620,14 +2851,14 @@
       </c>
       <c r="C46" s="10"/>
     </row>
-    <row r="47" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
     </row>
-    <row r="48" spans="1:12" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Cập nhật Đại Hoàng - Hoa Lư - Bái Dính
</commit_message>
<xml_diff>
--- a/Data_HDDT.xlsx
+++ b/Data_HDDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E4028E8-A79E-48CA-8FFB-1B074B1F8EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD6957D-7D0D-403E-8C3B-7B08EC4D94B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="345">
   <si>
     <t>Mã kho</t>
   </si>
@@ -997,6 +997,81 @@
   </si>
   <si>
     <t>HH050-19</t>
+  </si>
+  <si>
+    <t>HH050-030</t>
+  </si>
+  <si>
+    <t>Đại Hoàng</t>
+  </si>
+  <si>
+    <t>KDNL178</t>
+  </si>
+  <si>
+    <t>KDNL078</t>
+  </si>
+  <si>
+    <t>HH007044</t>
+  </si>
+  <si>
+    <t>HH009-001</t>
+  </si>
+  <si>
+    <t>HH050-034</t>
+  </si>
+  <si>
+    <t>HH0638</t>
+  </si>
+  <si>
+    <t>1K25TDH</t>
+  </si>
+  <si>
+    <t>Hoa Lư</t>
+  </si>
+  <si>
+    <t>KDNL179</t>
+  </si>
+  <si>
+    <t>KDNL079</t>
+  </si>
+  <si>
+    <t>HH007043</t>
+  </si>
+  <si>
+    <t>HH009-003</t>
+  </si>
+  <si>
+    <t>HH050-033</t>
+  </si>
+  <si>
+    <t>HH0639</t>
+  </si>
+  <si>
+    <t>1K25THL</t>
+  </si>
+  <si>
+    <t>Bái Đính</t>
+  </si>
+  <si>
+    <t>KDNL177</t>
+  </si>
+  <si>
+    <t>KDNL077</t>
+  </si>
+  <si>
+    <t>HH007042</t>
+  </si>
+  <si>
+    <t>HH009-002</t>
+  </si>
+  <si>
+    <t>HH050-032</t>
+  </si>
+  <si>
+    <t>HH06370</t>
+  </si>
+  <si>
+    <t>1K25TBD</t>
   </si>
 </sst>
 </file>
@@ -1488,16 +1563,17 @@
   <dimension ref="A2:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
@@ -2737,6 +2813,9 @@
       <c r="G38" s="4" t="s">
         <v>191</v>
       </c>
+      <c r="H38" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="I38" s="1" t="s">
         <v>233</v>
       </c>
@@ -2792,7 +2871,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>11</v>
       </c>
@@ -2800,15 +2879,66 @@
         <v>333115</v>
       </c>
       <c r="C40" s="10"/>
-      <c r="D40" s="4"/>
+      <c r="D40" s="4" t="s">
+        <v>321</v>
+      </c>
       <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="F40" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="41" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
+      <c r="D41" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="42" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
@@ -2816,6 +2946,33 @@
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
+      <c r="D42" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="43" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">

</xml_diff>

<commit_message>
Cập nhật mã thuế, dải hd 2026
</commit_message>
<xml_diff>
--- a/Data_HDDT.xlsx
+++ b/Data_HDDT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD6957D-7D0D-403E-8C3B-7B08EC4D94B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C793F33-DF8F-4BD6-8A84-2E94B36CD082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nhap lieu" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="348">
   <si>
     <t>Mã kho</t>
   </si>
@@ -93,9 +93,6 @@
     <t>KDNL005</t>
   </si>
   <si>
-    <t>1K25TCH</t>
-  </si>
-  <si>
     <t>Nam Định</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>KDNL006</t>
   </si>
   <si>
-    <t>1K25TDA</t>
-  </si>
-  <si>
     <t>HH050</t>
   </si>
   <si>
@@ -204,9 +198,6 @@
     <t>KDNL053</t>
   </si>
   <si>
-    <t>1K25THV</t>
-  </si>
-  <si>
     <t>Hồng Sơn</t>
   </si>
   <si>
@@ -237,9 +228,6 @@
     <t>KDNL063</t>
   </si>
   <si>
-    <t>1K25THU</t>
-  </si>
-  <si>
     <t>Khánh Hòa</t>
   </si>
   <si>
@@ -282,9 +270,6 @@
     <t>HH050-8</t>
   </si>
   <si>
-    <t>1K25TLP</t>
-  </si>
-  <si>
     <t>Liên Minh</t>
   </si>
   <si>
@@ -330,9 +315,6 @@
     <t>KDNL051</t>
   </si>
   <si>
-    <t>1K25TLA</t>
-  </si>
-  <si>
     <t>Lộc Hạ</t>
   </si>
   <si>
@@ -348,9 +330,6 @@
     <t>KDNL004</t>
   </si>
   <si>
-    <t>1K25TLH</t>
-  </si>
-  <si>
     <t>Mã thuế</t>
   </si>
   <si>
@@ -384,9 +363,6 @@
     <t>KDNL003</t>
   </si>
   <si>
-    <t>1K25TMX</t>
-  </si>
-  <si>
     <t>Nam Hồng</t>
   </si>
   <si>
@@ -402,9 +378,6 @@
     <t>KDNL018</t>
   </si>
   <si>
-    <t>1K25TNH</t>
-  </si>
-  <si>
     <t>Nam Vân</t>
   </si>
   <si>
@@ -459,9 +432,6 @@
     <t>HH009NG</t>
   </si>
   <si>
-    <t>1K25TNG</t>
-  </si>
-  <si>
     <t>Phủ Lý</t>
   </si>
   <si>
@@ -477,9 +447,6 @@
     <t>HH050-9</t>
   </si>
   <si>
-    <t>1K25TPL</t>
-  </si>
-  <si>
     <t>Quảng Trường</t>
   </si>
   <si>
@@ -492,9 +459,6 @@
     <t>HH009007</t>
   </si>
   <si>
-    <t>1K25TQT</t>
-  </si>
-  <si>
     <t>Song Hào</t>
   </si>
   <si>
@@ -513,9 +477,6 @@
     <t>KDNL065</t>
   </si>
   <si>
-    <t>1K25TSH</t>
-  </si>
-  <si>
     <t>Tam Điệp</t>
   </si>
   <si>
@@ -531,9 +492,6 @@
     <t>HH050-10</t>
   </si>
   <si>
-    <t>1K25TTD</t>
-  </si>
-  <si>
     <t>Tân Thành</t>
   </si>
   <si>
@@ -573,9 +531,6 @@
     <t>KHO4</t>
   </si>
   <si>
-    <t>1K25TNB</t>
-  </si>
-  <si>
     <t>Tràng An</t>
   </si>
   <si>
@@ -780,99 +735,39 @@
     <t>KDNL017</t>
   </si>
   <si>
-    <t>1K25TLD</t>
-  </si>
-  <si>
-    <t>1K25TVP</t>
-  </si>
-  <si>
     <t>HH050-022</t>
   </si>
   <si>
-    <t>1K25TBX</t>
-  </si>
-  <si>
-    <t>1K25TML</t>
-  </si>
-  <si>
-    <t>1K25TNC</t>
-  </si>
-  <si>
-    <t>1K25TTP</t>
-  </si>
-  <si>
-    <t>1K25TXT</t>
-  </si>
-  <si>
-    <t>1K25TTS</t>
-  </si>
-  <si>
-    <t>1K25TGT</t>
-  </si>
-  <si>
-    <t>1K25TGX</t>
-  </si>
-  <si>
-    <t>1K25TLM</t>
-  </si>
-  <si>
-    <t>1K25TNV</t>
-  </si>
-  <si>
-    <t>1K25TTA</t>
-  </si>
-  <si>
-    <t>1K25TTR</t>
-  </si>
-  <si>
     <t>KDNL172</t>
   </si>
   <si>
     <t>KDNL170</t>
   </si>
   <si>
-    <t>1K25TNP</t>
-  </si>
-  <si>
     <t>KDNL176</t>
   </si>
   <si>
     <t>KDNL159</t>
   </si>
   <si>
-    <t>1K25TAB</t>
-  </si>
-  <si>
     <t>KDNL174</t>
   </si>
   <si>
     <t>KDNL107</t>
   </si>
   <si>
-    <t>1K25THS</t>
-  </si>
-  <si>
     <t>KDNL109</t>
   </si>
   <si>
-    <t>1K25TAC</t>
-  </si>
-  <si>
     <t>KDNL158</t>
   </si>
   <si>
-    <t>1K25TKN</t>
-  </si>
-  <si>
     <t>KDNL119</t>
   </si>
   <si>
     <t>KDNL157</t>
   </si>
   <si>
-    <t>1K25TAA</t>
-  </si>
-  <si>
     <t>KDNL156</t>
   </si>
   <si>
@@ -891,9 +786,6 @@
     <t>KDNL171</t>
   </si>
   <si>
-    <t>1K25TTT</t>
-  </si>
-  <si>
     <t>KDNL155</t>
   </si>
   <si>
@@ -1023,9 +915,6 @@
     <t>HH0638</t>
   </si>
   <si>
-    <t>1K25TDH</t>
-  </si>
-  <si>
     <t>Hoa Lư</t>
   </si>
   <si>
@@ -1047,9 +936,6 @@
     <t>HH0639</t>
   </si>
   <si>
-    <t>1K25THL</t>
-  </si>
-  <si>
     <t>Bái Đính</t>
   </si>
   <si>
@@ -1071,7 +957,130 @@
     <t>HH06370</t>
   </si>
   <si>
-    <t>1K25TBD</t>
+    <t>1K26TBX</t>
+  </si>
+  <si>
+    <t>1K26TCH</t>
+  </si>
+  <si>
+    <t>1K26TDA</t>
+  </si>
+  <si>
+    <t>1K26TNP</t>
+  </si>
+  <si>
+    <t>1K26TTS</t>
+  </si>
+  <si>
+    <t>1K26TAB</t>
+  </si>
+  <si>
+    <t>1K26TGX</t>
+  </si>
+  <si>
+    <t>1K26TGT</t>
+  </si>
+  <si>
+    <t>1K26THV</t>
+  </si>
+  <si>
+    <t>1K26THS</t>
+  </si>
+  <si>
+    <t>1K26THU</t>
+  </si>
+  <si>
+    <t>1K26TAC</t>
+  </si>
+  <si>
+    <t>1K26TKN</t>
+  </si>
+  <si>
+    <t>1K26TLP</t>
+  </si>
+  <si>
+    <t>1K26TLM</t>
+  </si>
+  <si>
+    <t>1K26TLD</t>
+  </si>
+  <si>
+    <t>1K26TLA</t>
+  </si>
+  <si>
+    <t>1K26TLH</t>
+  </si>
+  <si>
+    <t>1K26TML</t>
+  </si>
+  <si>
+    <t>1K26TMX</t>
+  </si>
+  <si>
+    <t>1K26TNH</t>
+  </si>
+  <si>
+    <t>1K26TNV</t>
+  </si>
+  <si>
+    <t>1K26TAA</t>
+  </si>
+  <si>
+    <t>1K26TNC</t>
+  </si>
+  <si>
+    <t>1K26TNG</t>
+  </si>
+  <si>
+    <t>1K26TPL</t>
+  </si>
+  <si>
+    <t>1K26TQT</t>
+  </si>
+  <si>
+    <t>1K26TSH</t>
+  </si>
+  <si>
+    <t>1K26TTD</t>
+  </si>
+  <si>
+    <t>1K26TTT</t>
+  </si>
+  <si>
+    <t>1K26TTP</t>
+  </si>
+  <si>
+    <t>1K26TNB</t>
+  </si>
+  <si>
+    <t>1K26TTA</t>
+  </si>
+  <si>
+    <t>1K26TTR</t>
+  </si>
+  <si>
+    <t>1K26TVP</t>
+  </si>
+  <si>
+    <t>1K26TXT</t>
+  </si>
+  <si>
+    <t>1K26TDH</t>
+  </si>
+  <si>
+    <t>1K26THL</t>
+  </si>
+  <si>
+    <t>1K26TBD</t>
+  </si>
+  <si>
+    <t>Gia Tường</t>
+  </si>
+  <si>
+    <t>1K26TAD</t>
+  </si>
+  <si>
+    <t>HH050-037</t>
   </si>
 </sst>
 </file>
@@ -1560,42 +1569,42 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:M55"/>
+  <dimension ref="A2:P55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K43" sqref="K43"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="9.9" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
-    <col min="10" max="390" width="8.42578125" style="1" customWidth="1"/>
-    <col min="391" max="16384" width="8.42578125" style="1"/>
+    <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
+    <col min="10" max="390" width="8.44140625" style="1" customWidth="1"/>
+    <col min="391" max="16384" width="8.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E2" s="1" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>0</v>
@@ -1607,19 +1616,19 @@
         <v>2</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1637,27 +1646,27 @@
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>319</v>
+        <v>283</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>262</v>
+        <v>233</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>250</v>
+        <v>306</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -1675,24 +1684,24 @@
         <v>16</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>18</v>
+        <v>307</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -1701,842 +1710,858 @@
         <v>12</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="I6" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="D7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="H7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="I7" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="H8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="D9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="H9" s="6" t="s">
-        <v>318</v>
+        <v>282</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>267</v>
+        <v>311</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="B10" s="6">
         <v>1000</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="I10" s="1" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>268</v>
+        <v>237</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>257</v>
+        <v>312</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="B11" s="6">
         <v>1900</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="I11" s="1" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>256</v>
+        <v>313</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" s="6" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="B12" s="6">
         <v>2000</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="I12" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="K12" s="6" t="s">
-        <v>55</v>
+        <v>314</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="6" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="B13" s="6">
         <v>1000</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="I13" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="H14" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="I14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="J14" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="K14" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:16" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="J14" s="6" t="s">
+      <c r="F15" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="G15" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="4" t="s">
+      <c r="H15" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="I15" s="1" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>271</v>
+        <v>239</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>272</v>
+        <v>317</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="D16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="4" t="s">
+      <c r="H17" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="I17" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="G18" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="K17" s="1" t="s">
+      <c r="H18" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="H19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="4" t="s">
+      <c r="I19" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="4" t="s">
+      <c r="I20" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="K20" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="G21" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="H21" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="K21" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="B22" s="1">
         <v>8</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="H23" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="I23" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="K23" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="H24" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="K24" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="J23" s="1" t="s">
+      <c r="E25" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="F25" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="L23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="H25" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>117</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12" t="s">
-        <v>126</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="4" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>277</v>
+        <v>328</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="4" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>252</v>
+        <v>329</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="4" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>279</v>
+        <v>244</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>140</v>
+        <v>330</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="10">
         <v>131111</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="4" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>146</v>
+        <v>331</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B30" s="10">
         <v>131112</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="4" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>150</v>
+        <v>139</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>347</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>151</v>
+        <v>332</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>11</v>
       </c>
@@ -2545,146 +2570,146 @@
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="4" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>158</v>
+        <v>333</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="4" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>164</v>
+        <v>334</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" s="10">
         <v>51111</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="4" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>284</v>
+        <v>335</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B34" s="10">
         <v>51115</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>285</v>
+        <v>249</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>253</v>
+        <v>336</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>11</v>
       </c>
@@ -2693,185 +2718,185 @@
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="4" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>178</v>
+        <v>337</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B36" s="10">
-        <v>6321</v>
+        <v>63211</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="4" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>260</v>
+        <v>338</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="J37" s="1" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>261</v>
+        <v>339</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38" s="10">
         <v>333111</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="4" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>320</v>
+        <v>284</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>248</v>
+        <v>340</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B39" s="10">
         <v>333112</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="4" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>317</v>
+        <v>281</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>254</v>
+        <v>341</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>11</v>
       </c>
@@ -2880,126 +2905,135 @@
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="4" t="s">
-        <v>321</v>
+        <v>285</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4" t="s">
-        <v>324</v>
+        <v>288</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>325</v>
+        <v>289</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>326</v>
+        <v>290</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>327</v>
+        <v>291</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>322</v>
+        <v>286</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>328</v>
+        <v>342</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="1" t="s">
-        <v>329</v>
+        <v>292</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>332</v>
+        <v>295</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>333</v>
+        <v>296</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>334</v>
+        <v>297</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>335</v>
+        <v>298</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>330</v>
+        <v>293</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="1" t="s">
-        <v>337</v>
+        <v>299</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>340</v>
+        <v>302</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>341</v>
+        <v>303</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>342</v>
+        <v>304</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>344</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
-    </row>
-    <row r="44" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D43" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B44" s="10">
         <v>131111</v>
       </c>
       <c r="C44" s="10"/>
     </row>
-    <row r="45" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B45" s="10">
         <v>131112</v>
       </c>
       <c r="C45" s="10"/>
     </row>
-    <row r="46" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>11</v>
       </c>
@@ -3008,32 +3042,32 @@
       </c>
       <c r="C46" s="10"/>
     </row>
-    <row r="47" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
     </row>
-    <row r="48" spans="1:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B48" s="10">
         <v>3338111</v>
       </c>
       <c r="C48" s="10"/>
     </row>
-    <row r="49" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B49" s="10">
         <v>3338121</v>
       </c>
       <c r="C49" s="10"/>
     </row>
-    <row r="50" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>11</v>
       </c>
@@ -3042,41 +3076,41 @@
       </c>
       <c r="C50" s="10"/>
     </row>
-    <row r="51" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B51" s="10">
-        <v>6321</v>
+        <v>63211</v>
       </c>
       <c r="C51" s="10"/>
     </row>
-    <row r="52" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
     </row>
-    <row r="53" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B53" s="10">
         <v>333111</v>
       </c>
       <c r="C53" s="10"/>
     </row>
-    <row r="54" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B54" s="10">
         <v>333112</v>
       </c>
       <c r="C54" s="10"/>
     </row>
-    <row r="55" spans="1:3" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>11</v>
       </c>

</xml_diff>